<commit_message>
Set envionemnent in the cyress.config file and updated all module scripts
</commit_message>
<xml_diff>
--- a/cypress/fixtures/LoginData.xlsx
+++ b/cypress/fixtures/LoginData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -28,30 +28,9 @@
     <t>Password</t>
   </si>
   <si>
-    <t>dfhtestuser@gmail.com</t>
-  </si>
-  <si>
-    <t>dfh@88741</t>
-  </si>
-  <si>
     <t>User Id</t>
   </si>
   <si>
-    <t>precious.reindeer.bxff@flashpost.net</t>
-  </si>
-  <si>
-    <t>p@sS1234</t>
-  </si>
-  <si>
-    <t>pleased.aardwolf.zfwv@flashpost.net</t>
-  </si>
-  <si>
-    <t>certain.mackerel.cjtg@flashpost.net</t>
-  </si>
-  <si>
-    <t>steady.halibut.nvlx@flashpost.net</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -61,20 +40,35 @@
     <t>Invalid User</t>
   </si>
   <si>
-    <t>rizwikhattak@gmail.com</t>
-  </si>
-  <si>
     <t>pakistan@1234</t>
   </si>
   <si>
     <t>rizwikhattak43@gmail.com</t>
+  </si>
+  <si>
+    <t>KE#S3bF%9gau</t>
+  </si>
+  <si>
+    <t>rM{5Q#d&amp;T4FB</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Stagging</t>
+  </si>
+  <si>
+    <t>rizwikhattak77@gmail.com</t>
+  </si>
+  <si>
+    <t>shakeebqau@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +98,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F4350"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -126,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -148,6 +148,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -442,11 +445,12 @@
     <col min="2" max="2" width="36.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="24.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -455,126 +459,95 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    <row r="4" spans="1:5">
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="6"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="6"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="6"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
     </row>
@@ -597,20 +570,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
-    <hyperlink ref="B5" r:id="rId7"/>
-    <hyperlink ref="C5" r:id="rId8"/>
-    <hyperlink ref="B6" r:id="rId9"/>
-    <hyperlink ref="C6" r:id="rId10"/>
-    <hyperlink ref="B7" r:id="rId11"/>
-    <hyperlink ref="C7" r:id="rId12"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3" display="p@sS1234"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -632,7 +596,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -641,7 +605,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -649,13 +613,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>